<commit_message>
Implementaçaõ do vizinho mais próximo pseudo-aleatório e atualizaçaõ dos resultados do graspRVND
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/Comparações dos valores de alfa para o graspRVND.xlsx
+++ b/Arquivos/Comparações/Comparações dos valores de alfa para o graspRVND.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="51">
   <si>
     <t>Valores de α</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>gr21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
   </si>
   <si>
     <t>gr24</t>
@@ -177,11 +174,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -206,8 +203,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,15 +227,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,7 +249,77 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,91 +334,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,19 +356,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,127 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,19 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,6 +477,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,6 +565,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -592,47 +634,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -651,17 +652,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,152 +667,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -828,20 +825,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1164,8 +1155,8 @@
   <sheetPr/>
   <dimension ref="C3:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1174,15 +1165,18 @@
     <col min="3" max="3" width="11.1428571428571" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.1428571428571" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" style="1"/>
-    <col min="6" max="9" width="9.14285714285714" style="1"/>
+    <col min="6" max="7" width="9.14285714285714" style="1"/>
+    <col min="8" max="8" width="11.7142857142857" style="1"/>
+    <col min="9" max="9" width="9.14285714285714" style="1"/>
     <col min="10" max="10" width="10.2857142857143" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.1428571428571" style="1" customWidth="1"/>
     <col min="12" max="14" width="11.7142857142857" style="1"/>
-    <col min="15" max="16" width="9.14285714285714" style="1"/>
+    <col min="15" max="15" width="10.7142857142857" style="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="1"/>
     <col min="17" max="17" width="10.2857142857143" style="1" customWidth="1"/>
     <col min="18" max="18" width="19.1428571428571" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.7142857142857" style="1"/>
-    <col min="22" max="16384" width="9.14285714285714" style="1"/>
+    <col min="19" max="22" width="11.7142857142857" style="1"/>
+    <col min="23" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="3" ht="15.75" spans="3:22">
@@ -1277,13 +1271,15 @@
       <c r="E5" s="4">
         <v>649.82</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>657.9</v>
       </c>
       <c r="G5" s="4">
         <v>711.77</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="5">
+        <v>734.28</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1293,29 +1289,33 @@
       <c r="L5" s="4">
         <v>1289.94</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>1368.02</v>
       </c>
       <c r="N5" s="4">
         <v>1344.31</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="5">
+        <v>1331.65</v>
+      </c>
       <c r="Q5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="R5" s="6">
         <v>210</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="4">
         <v>1953.66</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="4">
         <v>1954.31</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="4">
         <v>1933.82</v>
       </c>
-      <c r="V5" s="2"/>
+      <c r="V5" s="5">
+        <v>1916.99</v>
+      </c>
     </row>
     <row r="6" ht="15.75" spans="3:22">
       <c r="C6" s="3" t="s">
@@ -1327,13 +1327,15 @@
       <c r="E6" s="4">
         <v>275</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>271</v>
       </c>
       <c r="G6" s="4">
         <v>246</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="5">
+        <v>268</v>
+      </c>
       <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1343,29 +1345,33 @@
       <c r="L6" s="4">
         <v>581</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>571</v>
       </c>
       <c r="N6" s="4">
         <v>571</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" s="5">
+        <v>546</v>
+      </c>
       <c r="Q6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="R6" s="6">
         <v>21</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="4">
         <v>1035</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="4">
         <v>918</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="4">
         <v>918</v>
       </c>
-      <c r="V6" s="2"/>
+      <c r="V6" s="5">
+        <v>939</v>
+      </c>
     </row>
     <row r="7" ht="15.75" spans="3:22">
       <c r="C7" s="3" t="s">
@@ -1377,13 +1383,15 @@
       <c r="E7" s="4">
         <v>319</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>282</v>
       </c>
       <c r="G7" s="4">
         <v>282</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="5">
+        <v>282</v>
+      </c>
       <c r="J7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1393,29 +1401,33 @@
       <c r="L7" s="4">
         <v>692</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>651</v>
       </c>
       <c r="N7" s="4">
         <v>640</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="5">
+        <v>651</v>
+      </c>
       <c r="Q7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R7" s="6">
         <v>21</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7" s="4">
         <v>1090</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="4">
         <v>1086</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7" s="4">
         <v>1090</v>
       </c>
-      <c r="V7" s="2"/>
+      <c r="V7" s="5">
+        <v>1090</v>
+      </c>
     </row>
     <row r="8" ht="15.75" spans="3:22">
       <c r="C8" s="3" t="s">
@@ -1427,13 +1439,15 @@
       <c r="E8" s="4">
         <v>480.48</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>480.48</v>
       </c>
       <c r="G8" s="4">
         <v>480.48</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="5">
+        <v>480.48</v>
+      </c>
       <c r="J8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1443,29 +1457,33 @@
       <c r="L8" s="4">
         <v>1749.38</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>1733.82</v>
       </c>
       <c r="N8" s="4">
         <v>1733.82</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="5">
+        <v>1733.82</v>
+      </c>
       <c r="Q8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="R8" s="6">
         <v>39</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8" s="4">
         <v>3910.64</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="4">
         <v>3868.97</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="4">
         <v>3859.81</v>
       </c>
-      <c r="V8" s="2"/>
+      <c r="V8" s="5">
+        <v>3910.64</v>
+      </c>
     </row>
     <row r="9" ht="15.75" spans="3:22">
       <c r="C9" s="3" t="s">
@@ -1477,13 +1495,15 @@
       <c r="E9" s="4">
         <v>10301.6</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>9682.94</v>
       </c>
       <c r="G9" s="4">
         <v>9776.1</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="5">
+        <v>9776.1</v>
+      </c>
       <c r="J9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1493,29 +1513,33 @@
       <c r="L9" s="4">
         <v>25935.45</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="4">
         <v>26660.41</v>
       </c>
       <c r="N9" s="4">
         <v>25378.24</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="5">
+        <v>26472</v>
+      </c>
       <c r="Q9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="6">
         <v>95</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9" s="4">
         <v>51268.42</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="4">
         <v>50491.65</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9" s="4">
         <v>49999.6</v>
       </c>
-      <c r="V9" s="2"/>
+      <c r="V9" s="5">
+        <v>50047.08</v>
+      </c>
     </row>
     <row r="10" ht="15.75" spans="3:22">
       <c r="C10" s="3" t="s">
@@ -1527,13 +1551,15 @@
       <c r="E10" s="4">
         <v>224.88</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>224.88</v>
       </c>
       <c r="G10" s="4">
         <v>224.88</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="5">
+        <v>224.88</v>
+      </c>
       <c r="J10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1543,29 +1569,33 @@
       <c r="L10" s="4">
         <v>1140.19</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="4">
         <v>1140.19</v>
       </c>
       <c r="N10" s="4">
         <v>1140.19</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="5">
+        <v>966.37</v>
+      </c>
       <c r="Q10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="R10" s="6">
         <v>10</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="4">
         <v>1637.31</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="4">
         <v>1637.31</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10" s="4">
         <v>1637.31</v>
       </c>
-      <c r="V10" s="2"/>
+      <c r="V10" s="5">
+        <v>1528.5</v>
+      </c>
     </row>
     <row r="11" ht="15.75" spans="3:22">
       <c r="C11" s="3" t="s">
@@ -1577,13 +1607,15 @@
       <c r="E11" s="4">
         <v>1123.61</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>1068.23</v>
       </c>
       <c r="G11" s="4">
         <v>1029.79</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="5">
+        <v>1038.42</v>
+      </c>
       <c r="J11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1593,29 +1625,33 @@
       <c r="L11" s="4">
         <v>2390.07</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="4">
         <v>2605.19</v>
       </c>
       <c r="N11" s="4">
         <v>2400.43</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="5">
+        <v>2505.41</v>
+      </c>
       <c r="Q11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="R11" s="6">
         <v>97</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11" s="4">
         <v>3828.1</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="4">
         <v>3861.47</v>
       </c>
-      <c r="U11" s="8">
+      <c r="U11" s="4">
         <v>3865.98</v>
       </c>
-      <c r="V11" s="2"/>
+      <c r="V11" s="5">
+        <v>3994.5</v>
+      </c>
     </row>
     <row r="12" ht="15.75" spans="3:22">
       <c r="C12" s="3" t="s">
@@ -1627,13 +1663,15 @@
       <c r="E12" s="4">
         <v>1297.97</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>1323.98</v>
       </c>
       <c r="G12" s="4">
         <v>1336.6</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="5">
+        <v>1337.23</v>
+      </c>
       <c r="J12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1643,29 +1681,33 @@
       <c r="L12" s="4">
         <v>2874.61</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>2898.38</v>
       </c>
       <c r="N12" s="4">
         <v>2803.38</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="5">
+        <v>2894.91</v>
+      </c>
       <c r="Q12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="R12" s="6">
         <v>112</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12" s="4">
         <v>4484.25</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="4">
         <v>4524.88</v>
       </c>
-      <c r="U12" s="8">
+      <c r="U12" s="4">
         <v>4503.43</v>
       </c>
-      <c r="V12" s="2"/>
+      <c r="V12" s="5">
+        <v>4547.13</v>
+      </c>
     </row>
     <row r="13" ht="15.75" spans="3:22">
       <c r="C13" s="3" t="s">
@@ -1677,13 +1719,15 @@
       <c r="E13" s="4">
         <v>99</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>98</v>
       </c>
       <c r="G13" s="4">
         <v>99</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="5">
+        <v>106</v>
+      </c>
       <c r="J13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1693,29 +1737,33 @@
       <c r="L13" s="4">
         <v>244</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="4">
         <v>220</v>
       </c>
       <c r="N13" s="4">
         <v>221</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="5">
+        <v>220</v>
+      </c>
       <c r="Q13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R13" s="6">
         <v>31</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13" s="4">
         <v>391</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="4">
         <v>388</v>
       </c>
-      <c r="U13" s="8">
+      <c r="U13" s="4">
         <v>392</v>
       </c>
-      <c r="V13" s="2"/>
+      <c r="V13" s="5">
+        <v>391</v>
+      </c>
     </row>
     <row r="14" ht="15.75" spans="3:22">
       <c r="C14" s="3" t="s">
@@ -1727,13 +1775,15 @@
       <c r="E14" s="4">
         <v>78.72</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>71.46</v>
       </c>
       <c r="G14" s="4">
         <v>71.46</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="5">
+        <v>72.9</v>
+      </c>
       <c r="J14" s="3" t="s">
         <v>16</v>
       </c>
@@ -1743,29 +1793,33 @@
       <c r="L14" s="4">
         <v>167.76</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="4">
         <v>168.63</v>
       </c>
       <c r="N14" s="4">
         <v>170.35</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="5">
+        <v>172.12</v>
+      </c>
       <c r="Q14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R14" s="6">
         <v>38</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S14" s="4">
         <v>282.97</v>
       </c>
-      <c r="T14" s="7">
+      <c r="T14" s="4">
         <v>281.57</v>
       </c>
-      <c r="U14" s="8">
+      <c r="U14" s="4">
         <v>281.59</v>
       </c>
-      <c r="V14" s="2"/>
+      <c r="V14" s="5">
+        <v>285.69</v>
+      </c>
     </row>
     <row r="15" ht="15.75" spans="3:22">
       <c r="C15" s="3" t="s">
@@ -1777,13 +1831,15 @@
       <c r="E15" s="4">
         <v>102.27</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>95.9</v>
       </c>
       <c r="G15" s="4">
         <v>98.03</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="5">
+        <v>97.1</v>
+      </c>
       <c r="J15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1793,29 +1849,33 @@
       <c r="L15" s="4">
         <v>215.67</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="4">
         <v>215.73</v>
       </c>
       <c r="N15" s="4">
         <v>220.05</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="5">
+        <v>217.06</v>
+      </c>
       <c r="Q15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="R15" s="6">
         <v>57</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15" s="4">
         <v>348.45</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="4">
         <v>340.57</v>
       </c>
-      <c r="U15" s="8">
+      <c r="U15" s="4">
         <v>335.91</v>
       </c>
-      <c r="V15" s="2"/>
+      <c r="V15" s="5">
+        <v>343.77</v>
+      </c>
     </row>
     <row r="16" ht="15.75" spans="3:22">
       <c r="C16" s="3" t="s">
@@ -1827,13 +1887,15 @@
       <c r="E16" s="4">
         <v>96.2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>96.2</v>
       </c>
       <c r="G16" s="4">
         <v>95.24</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="5">
+        <v>96.13</v>
+      </c>
       <c r="J16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1843,29 +1905,33 @@
       <c r="L16" s="4">
         <v>239.81</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="4">
         <v>232.34</v>
       </c>
       <c r="N16" s="4">
         <v>234.03</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="5">
+        <v>232.13</v>
+      </c>
       <c r="Q16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="R16" s="6">
         <v>75</v>
       </c>
-      <c r="S16" s="8">
+      <c r="S16" s="4">
         <v>402.32</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="4">
         <v>403.57</v>
       </c>
-      <c r="U16" s="8">
+      <c r="U16" s="4">
         <v>398.4</v>
       </c>
-      <c r="V16" s="2"/>
+      <c r="V16" s="5">
+        <v>395.33</v>
+      </c>
     </row>
     <row r="17" ht="15.75" spans="3:22">
       <c r="C17" s="3" t="s">
@@ -1877,13 +1943,15 @@
       <c r="E17" s="4">
         <v>145</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>145</v>
       </c>
       <c r="G17" s="4">
         <v>145</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="5">
+        <v>145</v>
+      </c>
       <c r="J17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1893,29 +1961,33 @@
       <c r="L17" s="4">
         <v>343</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="4">
         <v>317</v>
       </c>
       <c r="N17" s="4">
         <v>308</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="5">
+        <v>308</v>
+      </c>
       <c r="Q17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="R17" s="6">
         <v>19</v>
       </c>
-      <c r="S17" s="8">
+      <c r="S17" s="4">
         <v>521</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="4">
         <v>492</v>
       </c>
-      <c r="U17" s="8">
+      <c r="U17" s="4">
         <v>495</v>
       </c>
-      <c r="V17" s="2"/>
+      <c r="V17" s="5">
+        <v>492</v>
+      </c>
     </row>
     <row r="18" ht="15.75" spans="3:22">
       <c r="C18" s="3" t="s">
@@ -1927,13 +1999,15 @@
       <c r="E18" s="4">
         <v>497.77</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>493.84</v>
       </c>
       <c r="G18" s="4">
         <v>540.65</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="5">
+        <v>552.58</v>
+      </c>
       <c r="J18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1943,29 +2017,33 @@
       <c r="L18" s="4">
         <v>1036.7</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="4">
         <v>1027.2</v>
       </c>
       <c r="N18" s="4">
         <v>1057.68</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="5">
+        <v>1080.37</v>
+      </c>
       <c r="Q18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="R18" s="6">
         <v>196</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18" s="4">
         <v>1672.3</v>
       </c>
-      <c r="T18" s="7">
+      <c r="T18" s="4">
         <v>1632.51</v>
       </c>
-      <c r="U18" s="8">
+      <c r="U18" s="4">
         <v>1671.71</v>
       </c>
-      <c r="V18" s="2"/>
+      <c r="V18" s="5">
+        <v>1655.46</v>
+      </c>
     </row>
     <row r="19" ht="15.75" spans="3:22">
       <c r="C19" s="3" t="s">
@@ -1977,13 +2055,15 @@
       <c r="E19" s="4">
         <v>143</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>143</v>
       </c>
       <c r="G19" s="4">
         <v>143</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="5">
+        <v>143</v>
+      </c>
       <c r="J19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1993,29 +2073,33 @@
       <c r="L19" s="4">
         <v>359</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <v>359</v>
       </c>
       <c r="N19" s="4">
         <v>359</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="5">
+        <v>359</v>
+      </c>
       <c r="Q19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="R19" s="6">
         <v>12</v>
       </c>
-      <c r="S19" s="8">
+      <c r="S19" s="4">
         <v>640</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="4">
         <v>640</v>
       </c>
-      <c r="U19" s="8">
+      <c r="U19" s="4">
         <v>640</v>
       </c>
-      <c r="V19" s="2"/>
+      <c r="V19" s="5">
+        <v>640</v>
+      </c>
     </row>
     <row r="20" ht="15.75" spans="3:22">
       <c r="C20" s="3" t="s">
@@ -2027,14 +2111,14 @@
       <c r="E20" s="4">
         <v>181</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>181</v>
       </c>
       <c r="G20" s="4">
         <v>181</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>23</v>
+      <c r="H20" s="5">
+        <v>181</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>22</v>
@@ -2045,33 +2129,37 @@
       <c r="L20" s="4">
         <v>836</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="4">
         <v>727</v>
       </c>
       <c r="N20" s="4">
         <v>683</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="5">
+        <v>683</v>
+      </c>
       <c r="Q20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="R20" s="6">
         <v>15</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="4">
         <v>1276</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="4">
         <v>1276</v>
       </c>
-      <c r="U20" s="8">
+      <c r="U20" s="4">
         <v>1276</v>
       </c>
-      <c r="V20" s="2"/>
+      <c r="V20" s="5">
+        <v>1276</v>
+      </c>
     </row>
     <row r="21" ht="15.75" spans="3:22">
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="3">
         <v>6</v>
@@ -2079,15 +2167,17 @@
       <c r="E21" s="4">
         <v>162</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>162</v>
       </c>
       <c r="G21" s="4">
         <v>162</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="5">
+        <v>162</v>
+      </c>
       <c r="J21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K21" s="6">
         <v>12</v>
@@ -2095,33 +2185,37 @@
       <c r="L21" s="4">
         <v>413</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="4">
         <v>396</v>
       </c>
       <c r="N21" s="4">
         <v>396</v>
       </c>
-      <c r="O21" s="2"/>
+      <c r="O21" s="5">
+        <v>396</v>
+      </c>
       <c r="Q21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R21" s="6">
         <v>18</v>
       </c>
-      <c r="S21" s="8">
+      <c r="S21" s="4">
         <v>794</v>
       </c>
-      <c r="T21" s="7">
+      <c r="T21" s="4">
         <v>748</v>
       </c>
-      <c r="U21" s="8">
+      <c r="U21" s="4">
         <v>748</v>
       </c>
-      <c r="V21" s="2"/>
+      <c r="V21" s="5">
+        <v>749</v>
+      </c>
     </row>
     <row r="22" ht="15.75" spans="3:22">
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3">
         <v>12</v>
@@ -2129,15 +2223,17 @@
       <c r="E22" s="4">
         <v>558</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>558</v>
       </c>
       <c r="G22" s="4">
         <v>558</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="5">
+        <v>558</v>
+      </c>
       <c r="J22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K22" s="6">
         <v>24</v>
@@ -2145,33 +2241,37 @@
       <c r="L22" s="4">
         <v>1666</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="4">
         <v>1666</v>
       </c>
       <c r="N22" s="4">
         <v>1671</v>
       </c>
-      <c r="O22" s="2"/>
+      <c r="O22" s="5">
+        <v>1666</v>
+      </c>
       <c r="Q22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R22" s="6">
         <v>36</v>
       </c>
-      <c r="S22" s="8">
+      <c r="S22" s="4">
         <v>3059</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="4">
         <v>2992</v>
       </c>
-      <c r="U22" s="8">
+      <c r="U22" s="4">
         <v>2990</v>
       </c>
-      <c r="V22" s="2"/>
+      <c r="V22" s="5">
+        <v>2926</v>
+      </c>
     </row>
     <row r="23" ht="15.75" spans="3:22">
       <c r="C23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="3">
         <v>24</v>
@@ -2179,15 +2279,17 @@
       <c r="E23" s="4">
         <v>9270.86</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>9691.96</v>
       </c>
       <c r="G23" s="4">
         <v>9604.79</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="5">
+        <v>9855.29</v>
+      </c>
       <c r="J23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K23" s="6">
         <v>48</v>
@@ -2195,33 +2297,37 @@
       <c r="L23" s="4">
         <v>21333.83</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="4">
         <v>21588.21</v>
       </c>
       <c r="N23" s="4">
         <v>22297.67</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="O23" s="5">
+        <v>21724.12</v>
+      </c>
       <c r="Q23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R23" s="6">
         <v>72</v>
       </c>
-      <c r="S23" s="8">
+      <c r="S23" s="4">
         <v>32463.17</v>
       </c>
-      <c r="T23" s="7">
+      <c r="T23" s="4">
         <v>33412.45</v>
       </c>
-      <c r="U23" s="8">
+      <c r="U23" s="4">
         <v>33217.19</v>
       </c>
-      <c r="V23" s="2"/>
+      <c r="V23" s="5">
+        <v>32878.88</v>
+      </c>
     </row>
     <row r="24" ht="15.75" spans="3:22">
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3">
         <v>12</v>
@@ -2229,15 +2335,17 @@
       <c r="E24" s="4">
         <v>1954</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>2098</v>
       </c>
       <c r="G24" s="4">
         <v>1985</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="5">
+        <v>2122</v>
+      </c>
       <c r="J24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K24" s="6">
         <v>24</v>
@@ -2245,33 +2353,37 @@
       <c r="L24" s="4">
         <v>4013</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="4">
         <v>4043</v>
       </c>
       <c r="N24" s="4">
         <v>4024</v>
       </c>
-      <c r="O24" s="2"/>
+      <c r="O24" s="5">
+        <v>3990</v>
+      </c>
       <c r="Q24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R24" s="6">
         <v>36</v>
       </c>
-      <c r="S24" s="8">
+      <c r="S24" s="4">
         <v>6973</v>
       </c>
-      <c r="T24" s="7">
+      <c r="T24" s="4">
         <v>6814</v>
       </c>
-      <c r="U24" s="8">
+      <c r="U24" s="4">
         <v>6970</v>
       </c>
-      <c r="V24" s="2"/>
+      <c r="V24" s="5">
+        <v>6854</v>
+      </c>
     </row>
     <row r="25" ht="15.75" spans="3:22">
       <c r="C25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3">
         <v>25</v>
@@ -2279,15 +2391,17 @@
       <c r="E25" s="4">
         <v>4247.61</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>4304.35</v>
       </c>
       <c r="G25" s="4">
         <v>4605.12</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="5">
+        <v>4073.53</v>
+      </c>
       <c r="J25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K25" s="6">
         <v>50</v>
@@ -2295,33 +2409,37 @@
       <c r="L25" s="4">
         <v>8984.35</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="4">
         <v>8678.09</v>
       </c>
       <c r="N25" s="4">
         <v>9290.78</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="O25" s="5">
+        <v>8837.67</v>
+      </c>
       <c r="Q25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R25" s="6">
         <v>75</v>
       </c>
-      <c r="S25" s="8">
+      <c r="S25" s="4">
         <v>14043.38</v>
       </c>
-      <c r="T25" s="7">
+      <c r="T25" s="4">
         <v>14184.41</v>
       </c>
-      <c r="U25" s="8">
+      <c r="U25" s="4">
         <v>14123.96</v>
       </c>
-      <c r="V25" s="2"/>
+      <c r="V25" s="5">
+        <v>14480.5</v>
+      </c>
     </row>
     <row r="26" ht="15.75" spans="3:22">
       <c r="C26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="3">
         <v>37</v>
@@ -2329,15 +2447,17 @@
       <c r="E26" s="4">
         <v>5507.11</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>5270.34</v>
       </c>
       <c r="G26" s="4">
         <v>5943.72</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="5">
+        <v>5840.12</v>
+      </c>
       <c r="J26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K26" s="6">
         <v>75</v>
@@ -2345,33 +2465,37 @@
       <c r="L26" s="4">
         <v>11744.78</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="4">
         <v>11179.17</v>
       </c>
       <c r="N26" s="4">
         <v>11820.61</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="O26" s="5">
+        <v>11718.16</v>
+      </c>
       <c r="Q26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R26" s="6">
         <v>112</v>
       </c>
-      <c r="S26" s="8">
+      <c r="S26" s="4">
         <v>17822.55</v>
       </c>
-      <c r="T26" s="7">
+      <c r="T26" s="4">
         <v>18029.35</v>
       </c>
-      <c r="U26" s="8">
+      <c r="U26" s="4">
         <v>17898.34</v>
       </c>
-      <c r="V26" s="2"/>
+      <c r="V26" s="5">
+        <v>17757.85</v>
+      </c>
     </row>
     <row r="27" ht="15.75" spans="3:22">
       <c r="C27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="3">
         <v>50</v>
@@ -2379,15 +2503,17 @@
       <c r="E27" s="4">
         <v>6067.72</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>6065.16</v>
       </c>
       <c r="G27" s="4">
         <v>6723.24</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="5">
+        <v>6530.38</v>
+      </c>
       <c r="J27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K27" s="6">
         <v>100</v>
@@ -2395,33 +2521,37 @@
       <c r="L27" s="4">
         <v>13002.62</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="4">
         <v>13070.25</v>
       </c>
       <c r="N27" s="4">
         <v>13145.12</v>
       </c>
-      <c r="O27" s="2"/>
+      <c r="O27" s="5">
+        <v>12737.68</v>
+      </c>
       <c r="Q27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R27" s="6">
         <v>150</v>
       </c>
-      <c r="S27" s="8">
+      <c r="S27" s="4">
         <v>19869.87</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T27" s="4">
         <v>19996.33</v>
       </c>
-      <c r="U27" s="8">
+      <c r="U27" s="4">
         <v>20344.45</v>
       </c>
-      <c r="V27" s="2"/>
+      <c r="V27" s="5">
+        <v>20392.1</v>
+      </c>
     </row>
     <row r="28" ht="15.75" spans="3:22">
       <c r="C28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3">
         <v>25</v>
@@ -2429,15 +2559,17 @@
       <c r="E28" s="4">
         <v>3939.58</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>4241.03</v>
       </c>
       <c r="G28" s="4">
         <v>4120.85</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="5">
+        <v>4429.96</v>
+      </c>
       <c r="J28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K28" s="6">
         <v>50</v>
@@ -2445,33 +2577,37 @@
       <c r="L28" s="4">
         <v>8992.25</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="4">
         <v>9227.11</v>
       </c>
       <c r="N28" s="4">
         <v>9892.11</v>
       </c>
-      <c r="O28" s="2"/>
+      <c r="O28" s="5">
+        <v>9471.1</v>
+      </c>
       <c r="Q28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R28" s="6">
         <v>75</v>
       </c>
-      <c r="S28" s="8">
+      <c r="S28" s="4">
         <v>14492.68</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T28" s="4">
         <v>14337.91</v>
       </c>
-      <c r="U28" s="8">
+      <c r="U28" s="4">
         <v>14973.82</v>
       </c>
-      <c r="V28" s="2"/>
+      <c r="V28" s="5">
+        <v>14758.15</v>
+      </c>
     </row>
     <row r="29" ht="15.75" spans="3:22">
       <c r="C29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3">
         <v>37</v>
@@ -2479,15 +2615,17 @@
       <c r="E29" s="4">
         <v>5003.1</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>5258.74</v>
       </c>
       <c r="G29" s="4">
         <v>5128.61</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="5">
+        <v>5102.42</v>
+      </c>
       <c r="J29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K29" s="6">
         <v>75</v>
@@ -2495,33 +2633,37 @@
       <c r="L29" s="4">
         <v>11343.59</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="4">
         <v>11065.09</v>
       </c>
       <c r="N29" s="4">
         <v>11261.65</v>
       </c>
-      <c r="O29" s="2"/>
+      <c r="O29" s="5">
+        <v>11675.09</v>
+      </c>
       <c r="Q29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R29" s="6">
         <v>112</v>
       </c>
-      <c r="S29" s="8">
+      <c r="S29" s="4">
         <v>16864.39</v>
       </c>
-      <c r="T29" s="7">
+      <c r="T29" s="4">
         <v>16754.93</v>
       </c>
-      <c r="U29" s="8">
+      <c r="U29" s="4">
         <v>16935.49</v>
       </c>
-      <c r="V29" s="2"/>
+      <c r="V29" s="5">
+        <v>17202.36</v>
+      </c>
     </row>
     <row r="30" ht="15.75" spans="3:22">
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="3">
         <v>50</v>
@@ -2529,15 +2671,17 @@
       <c r="E30" s="4">
         <v>6086.05</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="4">
         <v>6123.04</v>
       </c>
       <c r="G30" s="4">
         <v>5997.25</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="5">
+        <v>6621.84</v>
+      </c>
       <c r="J30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K30" s="6">
         <v>100</v>
@@ -2545,33 +2689,37 @@
       <c r="L30" s="4">
         <v>12744.81</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30" s="4">
         <v>12653.32</v>
       </c>
       <c r="N30" s="4">
         <v>12752.49</v>
       </c>
-      <c r="O30" s="2"/>
+      <c r="O30" s="5">
+        <v>13420.52</v>
+      </c>
       <c r="Q30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R30" s="6">
         <v>150</v>
       </c>
-      <c r="S30" s="8">
+      <c r="S30" s="4">
         <v>20054.07</v>
       </c>
-      <c r="T30" s="7">
+      <c r="T30" s="4">
         <v>19843.62</v>
       </c>
-      <c r="U30" s="8">
+      <c r="U30" s="4">
         <v>19571.08</v>
       </c>
-      <c r="V30" s="2"/>
+      <c r="V30" s="5">
+        <v>19690.56</v>
+      </c>
     </row>
     <row r="31" ht="15.75" spans="3:22">
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="3">
         <v>25</v>
@@ -2579,15 +2727,17 @@
       <c r="E31" s="4">
         <v>4117.06</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>4021.19</v>
       </c>
       <c r="G31" s="4">
         <v>4180.94</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="5">
+        <v>4043.65</v>
+      </c>
       <c r="J31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K31" s="6">
         <v>50</v>
@@ -2595,33 +2745,37 @@
       <c r="L31" s="4">
         <v>9016.33</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="4">
         <v>8954.15</v>
       </c>
       <c r="N31" s="4">
         <v>8698.27</v>
       </c>
-      <c r="O31" s="2"/>
+      <c r="O31" s="5">
+        <v>9343.98</v>
+      </c>
       <c r="Q31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R31" s="6">
         <v>75</v>
       </c>
-      <c r="S31" s="8">
+      <c r="S31" s="4">
         <v>13692.78</v>
       </c>
-      <c r="T31" s="7">
+      <c r="T31" s="4">
         <v>13353.45</v>
       </c>
-      <c r="U31" s="8">
+      <c r="U31" s="4">
         <v>14148.87</v>
       </c>
-      <c r="V31" s="2"/>
+      <c r="V31" s="5">
+        <v>13636.48</v>
+      </c>
     </row>
     <row r="32" ht="15.75" spans="3:22">
       <c r="C32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="3">
         <v>25</v>
@@ -2629,15 +2783,17 @@
       <c r="E32" s="4">
         <v>3905.21</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <v>4040.31</v>
       </c>
       <c r="G32" s="4">
         <v>4289.94</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="5">
+        <v>4416.78</v>
+      </c>
       <c r="J32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" s="6">
         <v>50</v>
@@ -2645,33 +2801,37 @@
       <c r="L32" s="4">
         <v>8439.6</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="4">
         <v>8735.5</v>
       </c>
       <c r="N32" s="4">
         <v>8919.11</v>
       </c>
-      <c r="O32" s="2"/>
+      <c r="O32" s="5">
+        <v>9147.88</v>
+      </c>
       <c r="Q32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R32" s="6">
         <v>75</v>
       </c>
-      <c r="S32" s="8">
+      <c r="S32" s="4">
         <v>14289.5</v>
       </c>
-      <c r="T32" s="7">
+      <c r="T32" s="4">
         <v>13854.01</v>
       </c>
-      <c r="U32" s="8">
+      <c r="U32" s="4">
         <v>14809.93</v>
       </c>
-      <c r="V32" s="2"/>
+      <c r="V32" s="5">
+        <v>14206.08</v>
+      </c>
     </row>
     <row r="33" ht="15.75" spans="3:22">
       <c r="C33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="3">
         <v>25</v>
@@ -2679,15 +2839,17 @@
       <c r="E33" s="4">
         <v>3336.02</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="4">
         <v>3416.56</v>
       </c>
       <c r="G33" s="4">
         <v>3336.02</v>
       </c>
-      <c r="H33" s="2"/>
+      <c r="H33" s="5">
+        <v>3336.02</v>
+      </c>
       <c r="J33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K33" s="6">
         <v>50</v>
@@ -2695,33 +2857,37 @@
       <c r="L33" s="4">
         <v>8757.35</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="4">
         <v>9306.33</v>
       </c>
       <c r="N33" s="4">
         <v>9059.77</v>
       </c>
-      <c r="O33" s="2"/>
+      <c r="O33" s="5">
+        <v>9298.52</v>
+      </c>
       <c r="Q33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R33" s="6">
         <v>75</v>
       </c>
-      <c r="S33" s="8">
+      <c r="S33" s="4">
         <v>14587.97</v>
       </c>
-      <c r="T33" s="7">
+      <c r="T33" s="4">
         <v>14477.59</v>
       </c>
-      <c r="U33" s="8">
+      <c r="U33" s="4">
         <v>14569.5</v>
       </c>
-      <c r="V33" s="2"/>
+      <c r="V33" s="5">
+        <v>14361.97</v>
+      </c>
     </row>
     <row r="34" ht="15.75" spans="3:22">
       <c r="C34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D34" s="3">
         <v>26</v>
@@ -2729,15 +2895,17 @@
       <c r="E34" s="4">
         <v>2002.98</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="4">
         <v>2002.98</v>
       </c>
       <c r="G34" s="4">
         <v>2208.78</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="5">
+        <v>2381.41</v>
+      </c>
       <c r="J34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K34" s="6">
         <v>52</v>
@@ -2745,33 +2913,37 @@
       <c r="L34" s="4">
         <v>4605.86</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="4">
         <v>4648.13</v>
       </c>
       <c r="N34" s="4">
         <v>4685.06</v>
       </c>
-      <c r="O34" s="2"/>
+      <c r="O34" s="5">
+        <v>4658.88</v>
+      </c>
       <c r="Q34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R34" s="6">
         <v>78</v>
       </c>
-      <c r="S34" s="8">
+      <c r="S34" s="4">
         <v>8456.82</v>
       </c>
-      <c r="T34" s="7">
+      <c r="T34" s="4">
         <v>8572.94</v>
       </c>
-      <c r="U34" s="8">
+      <c r="U34" s="4">
         <v>8396.26</v>
       </c>
-      <c r="V34" s="2"/>
+      <c r="V34" s="5">
+        <v>8045.35</v>
+      </c>
     </row>
     <row r="35" ht="15.75" spans="3:22">
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="3">
         <v>79</v>
@@ -2779,15 +2951,17 @@
       <c r="E35" s="4">
         <v>7492.55</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <v>8775.59</v>
       </c>
       <c r="G35" s="4">
         <v>8939.88</v>
       </c>
-      <c r="H35" s="2"/>
+      <c r="H35" s="5">
+        <v>9154.38</v>
+      </c>
       <c r="J35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K35" s="6">
         <v>159</v>
@@ -2795,33 +2969,37 @@
       <c r="L35" s="4">
         <v>16861.76</v>
       </c>
-      <c r="M35" s="7">
+      <c r="M35" s="4">
         <v>17803.59</v>
       </c>
       <c r="N35" s="4">
         <v>16594.58</v>
       </c>
-      <c r="O35" s="2"/>
+      <c r="O35" s="5">
+        <v>16532.67</v>
+      </c>
       <c r="Q35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R35" s="6">
         <v>238</v>
       </c>
-      <c r="S35" s="8">
+      <c r="S35" s="4">
         <v>27341.07</v>
       </c>
-      <c r="T35" s="7">
+      <c r="T35" s="4">
         <v>27099.87</v>
       </c>
-      <c r="U35" s="8">
+      <c r="U35" s="4">
         <v>27788.54</v>
       </c>
-      <c r="V35" s="2"/>
+      <c r="V35" s="5">
+        <v>28495.83</v>
+      </c>
     </row>
     <row r="36" ht="15.75" spans="3:22">
       <c r="C36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3">
         <v>19</v>
@@ -2829,15 +3007,17 @@
       <c r="E36" s="4">
         <v>19642.8</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>20155.24</v>
       </c>
       <c r="G36" s="4">
         <v>18270.88</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="5">
+        <v>19041.59</v>
+      </c>
       <c r="J36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K36" s="6">
         <v>38</v>
@@ -2845,33 +3025,37 @@
       <c r="L36" s="4">
         <v>37105.79</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="4">
         <v>36936.72</v>
       </c>
       <c r="N36" s="4">
         <v>36658.25</v>
       </c>
-      <c r="O36" s="2"/>
+      <c r="O36" s="5">
+        <v>37235.52</v>
+      </c>
       <c r="Q36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R36" s="6">
         <v>57</v>
       </c>
-      <c r="S36" s="8">
+      <c r="S36" s="4">
         <v>59838.85</v>
       </c>
-      <c r="T36" s="7">
+      <c r="T36" s="4">
         <v>61124.68</v>
       </c>
-      <c r="U36" s="8">
+      <c r="U36" s="4">
         <v>63664.83</v>
       </c>
-      <c r="V36" s="2"/>
+      <c r="V36" s="5">
+        <v>62157.06</v>
+      </c>
     </row>
     <row r="37" ht="15.75" spans="3:22">
       <c r="C37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="3">
         <v>26</v>
@@ -2879,15 +3063,17 @@
       <c r="E37" s="4">
         <v>6733.38</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>6733.38</v>
       </c>
       <c r="G37" s="4">
         <v>6988.61</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="5">
+        <v>6988.61</v>
+      </c>
       <c r="J37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K37" s="6">
         <v>52</v>
@@ -2895,33 +3081,37 @@
       <c r="L37" s="4">
         <v>14703.61</v>
       </c>
-      <c r="M37" s="7">
+      <c r="M37" s="4">
         <v>14704.12</v>
       </c>
       <c r="N37" s="4">
         <v>14769.35</v>
       </c>
-      <c r="O37" s="2"/>
+      <c r="O37" s="5">
+        <v>14473.74</v>
+      </c>
       <c r="Q37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R37" s="6">
         <v>80</v>
       </c>
-      <c r="S37" s="8">
+      <c r="S37" s="4">
         <v>30488.7</v>
       </c>
-      <c r="T37" s="7">
+      <c r="T37" s="4">
         <v>29587.28</v>
       </c>
-      <c r="U37" s="8">
+      <c r="U37" s="4">
         <v>29524.41</v>
       </c>
-      <c r="V37" s="2"/>
+      <c r="V37" s="5">
+        <v>30116.09</v>
+      </c>
     </row>
     <row r="38" ht="15.75" spans="3:22">
       <c r="C38" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D38" s="3">
         <v>31</v>
@@ -2929,15 +3119,17 @@
       <c r="E38" s="4">
         <v>9378.8</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="4">
         <v>9329.87</v>
       </c>
       <c r="G38" s="4">
         <v>9284.41</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="5">
+        <v>9378.8</v>
+      </c>
       <c r="J38" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K38" s="6">
         <v>62</v>
@@ -2945,33 +3137,37 @@
       <c r="L38" s="4">
         <v>21566.03</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M38" s="4">
         <v>20818.9</v>
       </c>
       <c r="N38" s="4">
         <v>20911.81</v>
       </c>
-      <c r="O38" s="2"/>
+      <c r="O38" s="5">
+        <v>22712.56</v>
+      </c>
       <c r="Q38" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R38" s="6">
         <v>93</v>
       </c>
-      <c r="S38" s="8">
+      <c r="S38" s="4">
         <v>35368.11</v>
       </c>
-      <c r="T38" s="7">
+      <c r="T38" s="4">
         <v>36398.06</v>
       </c>
-      <c r="U38" s="8">
+      <c r="U38" s="4">
         <v>36785.95</v>
       </c>
-      <c r="V38" s="2"/>
+      <c r="V38" s="5">
+        <v>38249.99</v>
+      </c>
     </row>
     <row r="39" ht="15.75" spans="3:22">
       <c r="C39" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="3">
         <v>34</v>
@@ -2979,15 +3175,17 @@
       <c r="E39" s="4">
         <v>20168.23</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="4">
         <v>19998.88</v>
       </c>
       <c r="G39" s="4">
         <v>19894.6</v>
       </c>
-      <c r="H39" s="2"/>
+      <c r="H39" s="5">
+        <v>20389</v>
+      </c>
       <c r="J39" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K39" s="6">
         <v>68</v>
@@ -2995,33 +3193,37 @@
       <c r="L39" s="4">
         <v>44637.83</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="4">
         <v>44433.41</v>
       </c>
       <c r="N39" s="4">
         <v>44284.83</v>
       </c>
-      <c r="O39" s="2"/>
+      <c r="O39" s="5">
+        <v>44915.13</v>
+      </c>
       <c r="Q39" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R39" s="6">
         <v>102</v>
       </c>
-      <c r="S39" s="8">
+      <c r="S39" s="4">
         <v>67005.71</v>
       </c>
-      <c r="T39" s="7">
+      <c r="T39" s="4">
         <v>66781.21</v>
       </c>
-      <c r="U39" s="8">
+      <c r="U39" s="4">
         <v>66750.16</v>
       </c>
-      <c r="V39" s="2"/>
+      <c r="V39" s="5">
+        <v>67000.81</v>
+      </c>
     </row>
     <row r="40" ht="15.75" spans="3:22">
       <c r="C40" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3">
         <v>36</v>
@@ -3029,15 +3231,17 @@
       <c r="E40" s="4">
         <v>10742.86</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="4">
         <v>13256.11</v>
       </c>
       <c r="G40" s="4">
         <v>14069.99</v>
       </c>
-      <c r="H40" s="2"/>
+      <c r="H40" s="5">
+        <v>14816.48</v>
+      </c>
       <c r="J40" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K40" s="6">
         <v>72</v>
@@ -3045,33 +3249,37 @@
       <c r="L40" s="4">
         <v>26293.47</v>
       </c>
-      <c r="M40" s="7">
+      <c r="M40" s="4">
         <v>27812.24</v>
       </c>
       <c r="N40" s="4">
         <v>27196.57</v>
       </c>
-      <c r="O40" s="2"/>
+      <c r="O40" s="5">
+        <v>27374.48</v>
+      </c>
       <c r="Q40" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R40" s="6">
         <v>108</v>
       </c>
-      <c r="S40" s="8">
+      <c r="S40" s="4">
         <v>38203.84</v>
       </c>
-      <c r="T40" s="7">
+      <c r="T40" s="4">
         <v>38889.47</v>
       </c>
-      <c r="U40" s="8">
+      <c r="U40" s="4">
         <v>42179.7</v>
       </c>
-      <c r="V40" s="2"/>
+      <c r="V40" s="5">
+        <v>43050.36</v>
+      </c>
     </row>
     <row r="41" ht="15.75" spans="3:22">
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3">
         <v>38</v>
@@ -3079,15 +3287,17 @@
       <c r="E41" s="4">
         <v>14780.62</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="4">
         <v>18221.84</v>
       </c>
       <c r="G41" s="4">
         <v>17871.28</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="5">
+        <v>17619.52</v>
+      </c>
       <c r="J41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K41" s="6">
         <v>76</v>
@@ -3095,33 +3305,37 @@
       <c r="L41" s="4">
         <v>31161.21</v>
       </c>
-      <c r="M41" s="7">
+      <c r="M41" s="4">
         <v>30492.64</v>
       </c>
       <c r="N41" s="4">
         <v>30506.9</v>
       </c>
-      <c r="O41" s="2"/>
+      <c r="O41" s="5">
+        <v>31209.32</v>
+      </c>
       <c r="Q41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R41" s="6">
         <v>114</v>
       </c>
-      <c r="S41" s="8">
+      <c r="S41" s="4">
         <v>47013.52</v>
       </c>
-      <c r="T41" s="7">
+      <c r="T41" s="4">
         <v>48319.08</v>
       </c>
-      <c r="U41" s="8">
+      <c r="U41" s="4">
         <v>48489.8</v>
       </c>
-      <c r="V41" s="2"/>
+      <c r="V41" s="5">
+        <v>48364.89</v>
+      </c>
     </row>
     <row r="42" ht="15.75" spans="3:22">
       <c r="C42" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="3">
         <v>56</v>
@@ -3129,15 +3343,17 @@
       <c r="E42" s="4">
         <v>15824.06</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="4">
         <v>15849.71</v>
       </c>
       <c r="G42" s="4">
         <v>16664.97</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="5">
+        <v>16546.63</v>
+      </c>
       <c r="J42" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K42" s="6">
         <v>113</v>
@@ -3145,33 +3361,37 @@
       <c r="L42" s="4">
         <v>26272.2</v>
       </c>
-      <c r="M42" s="7">
+      <c r="M42" s="4">
         <v>34520.56</v>
       </c>
       <c r="N42" s="4">
         <v>31010.75</v>
       </c>
-      <c r="O42" s="2"/>
+      <c r="O42" s="5">
+        <v>30576.73</v>
+      </c>
       <c r="Q42" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R42" s="6">
         <v>169</v>
       </c>
-      <c r="S42" s="8">
+      <c r="S42" s="4">
         <v>46490.92</v>
       </c>
-      <c r="T42" s="7">
+      <c r="T42" s="4">
         <v>43792.8</v>
       </c>
-      <c r="U42" s="8">
+      <c r="U42" s="4">
         <v>45695.74</v>
       </c>
-      <c r="V42" s="2"/>
+      <c r="V42" s="5">
+        <v>45481.42</v>
+      </c>
     </row>
     <row r="43" ht="15.75" spans="3:22">
       <c r="C43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D43" s="3">
         <v>24</v>
@@ -3179,15 +3399,17 @@
       <c r="E43" s="4">
         <v>250.39</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="4">
         <v>246.96</v>
       </c>
       <c r="G43" s="4">
         <v>248.66</v>
       </c>
-      <c r="H43" s="2"/>
+      <c r="H43" s="5">
+        <v>257.43</v>
+      </c>
       <c r="J43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K43" s="6">
         <v>49</v>
@@ -3195,33 +3417,37 @@
       <c r="L43" s="4">
         <v>549.76</v>
       </c>
-      <c r="M43" s="7">
+      <c r="M43" s="4">
         <v>548.02</v>
       </c>
       <c r="N43" s="4">
         <v>535.33</v>
       </c>
-      <c r="O43" s="2"/>
+      <c r="O43" s="5">
+        <v>557.54</v>
+      </c>
       <c r="Q43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R43" s="6">
         <v>74</v>
       </c>
-      <c r="S43" s="8">
+      <c r="S43" s="4">
         <v>857.1</v>
       </c>
-      <c r="T43" s="7">
+      <c r="T43" s="4">
         <v>862.66</v>
       </c>
-      <c r="U43" s="8">
+      <c r="U43" s="4">
         <v>857.92</v>
       </c>
-      <c r="V43" s="2"/>
+      <c r="V43" s="5">
+        <v>872.04</v>
+      </c>
     </row>
     <row r="44" ht="15.75" spans="3:22">
       <c r="C44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="3">
         <v>48</v>
@@ -3229,15 +3455,17 @@
       <c r="E44" s="4">
         <v>563.96</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="4">
         <v>548.67</v>
       </c>
       <c r="G44" s="4">
         <v>541.57</v>
       </c>
-      <c r="H44" s="2"/>
+      <c r="H44" s="5">
+        <v>550.99</v>
+      </c>
       <c r="J44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K44" s="6">
         <v>97</v>
@@ -3245,33 +3473,37 @@
       <c r="L44" s="4">
         <v>1154.18</v>
       </c>
-      <c r="M44" s="7">
+      <c r="M44" s="4">
         <v>1165.33</v>
       </c>
       <c r="N44" s="4">
         <v>1140.86</v>
       </c>
-      <c r="O44" s="2"/>
+      <c r="O44" s="5">
+        <v>1158.27</v>
+      </c>
       <c r="Q44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R44" s="6">
         <v>146</v>
       </c>
-      <c r="S44" s="8">
+      <c r="S44" s="4">
         <v>1725.15</v>
       </c>
-      <c r="T44" s="7">
+      <c r="T44" s="4">
         <v>1733.09</v>
       </c>
-      <c r="U44" s="8">
+      <c r="U44" s="4">
         <v>1730.19</v>
       </c>
-      <c r="V44" s="2"/>
+      <c r="V44" s="5">
+        <v>1746.95</v>
+      </c>
     </row>
     <row r="45" ht="15.75" spans="3:22">
       <c r="C45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" s="3">
         <v>17</v>
@@ -3279,15 +3511,17 @@
       <c r="E45" s="4">
         <v>108.3</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>108.3</v>
       </c>
       <c r="G45" s="4">
         <v>108.3</v>
       </c>
-      <c r="H45" s="2"/>
+      <c r="H45" s="5">
+        <v>111.43</v>
+      </c>
       <c r="J45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K45" s="6">
         <v>35</v>
@@ -3295,33 +3529,37 @@
       <c r="L45" s="4">
         <v>269.28</v>
       </c>
-      <c r="M45" s="7">
+      <c r="M45" s="4">
         <v>253.82</v>
       </c>
       <c r="N45" s="4">
         <v>265.09</v>
       </c>
-      <c r="O45" s="2"/>
+      <c r="O45" s="5">
+        <v>254.17</v>
+      </c>
       <c r="Q45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R45" s="6">
         <v>52</v>
       </c>
-      <c r="S45" s="8">
+      <c r="S45" s="4">
         <v>422.36</v>
       </c>
-      <c r="T45" s="7">
+      <c r="T45" s="4">
         <v>435.08</v>
       </c>
-      <c r="U45" s="8">
+      <c r="U45" s="4">
         <v>429</v>
       </c>
-      <c r="V45" s="2"/>
+      <c r="V45" s="5">
+        <v>432.9</v>
+      </c>
     </row>
     <row r="46" ht="15.75" spans="3:22">
       <c r="C46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" s="3">
         <v>10</v>
@@ -3329,15 +3567,17 @@
       <c r="E46" s="4">
         <v>146</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="4">
         <v>146</v>
       </c>
       <c r="G46" s="4">
         <v>146</v>
       </c>
-      <c r="H46" s="2"/>
+      <c r="H46" s="5">
+        <v>150</v>
+      </c>
       <c r="J46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K46" s="6">
         <v>21</v>
@@ -3345,33 +3585,37 @@
       <c r="L46" s="4">
         <v>476</v>
       </c>
-      <c r="M46" s="7">
+      <c r="M46" s="4">
         <v>430</v>
       </c>
       <c r="N46" s="4">
         <v>418</v>
       </c>
-      <c r="O46" s="2"/>
+      <c r="O46" s="5">
+        <v>410</v>
+      </c>
       <c r="Q46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R46" s="6">
         <v>31</v>
       </c>
-      <c r="S46" s="8">
+      <c r="S46" s="4">
         <v>721</v>
       </c>
-      <c r="T46" s="7">
+      <c r="T46" s="4">
         <v>721</v>
       </c>
-      <c r="U46" s="8">
+      <c r="U46" s="4">
         <v>698</v>
       </c>
-      <c r="V46" s="2"/>
+      <c r="V46" s="5">
+        <v>698</v>
+      </c>
     </row>
     <row r="47" ht="15.75" spans="3:22">
       <c r="C47" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D47" s="3">
         <v>4</v>
@@ -3379,15 +3623,17 @@
       <c r="E47" s="4">
         <v>751.06</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="4">
         <v>751.06</v>
       </c>
       <c r="G47" s="4">
         <v>638.03</v>
       </c>
-      <c r="H47" s="2"/>
+      <c r="H47" s="5">
+        <v>638.03</v>
+      </c>
       <c r="J47" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K47" s="6">
         <v>8</v>
@@ -3395,33 +3641,37 @@
       <c r="L47" s="4">
         <v>1981.71</v>
       </c>
-      <c r="M47" s="7">
+      <c r="M47" s="4">
         <v>1981.71</v>
       </c>
       <c r="N47" s="4">
         <v>1397.42</v>
       </c>
-      <c r="O47" s="2"/>
+      <c r="O47" s="5">
+        <v>1397.42</v>
+      </c>
       <c r="Q47" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R47" s="6">
         <v>12</v>
       </c>
-      <c r="S47" s="8">
+      <c r="S47" s="4">
         <v>2741.1</v>
       </c>
-      <c r="T47" s="7">
+      <c r="T47" s="4">
         <v>2741.1</v>
       </c>
-      <c r="U47" s="8">
+      <c r="U47" s="4">
         <v>2731</v>
       </c>
-      <c r="V47" s="2"/>
+      <c r="V47" s="5">
+        <v>2731</v>
+      </c>
     </row>
     <row r="48" ht="15.75" spans="3:22">
       <c r="C48" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D48" s="3">
         <v>5</v>
@@ -3429,15 +3679,17 @@
       <c r="E48" s="4">
         <v>456.58</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="4">
         <v>456.58</v>
       </c>
       <c r="G48" s="4">
         <v>456.58</v>
       </c>
-      <c r="H48" s="2"/>
+      <c r="H48" s="5">
+        <v>456.58</v>
+      </c>
       <c r="J48" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K48" s="6">
         <v>11</v>
@@ -3445,29 +3697,33 @@
       <c r="L48" s="4">
         <v>2062.92</v>
       </c>
-      <c r="M48" s="7">
+      <c r="M48" s="4">
         <v>1684.93</v>
       </c>
       <c r="N48" s="4">
         <v>1591.34</v>
       </c>
-      <c r="O48" s="2"/>
+      <c r="O48" s="5">
+        <v>1647.33</v>
+      </c>
       <c r="Q48" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R48" s="6">
         <v>16</v>
       </c>
-      <c r="S48" s="8">
+      <c r="S48" s="4">
         <v>2540.07</v>
       </c>
-      <c r="T48" s="7">
+      <c r="T48" s="4">
         <v>2540.07</v>
       </c>
-      <c r="U48" s="8">
+      <c r="U48" s="4">
         <v>2540.07</v>
       </c>
-      <c r="V48" s="2"/>
+      <c r="V48" s="5">
+        <v>2540.07</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>